<commit_message>
Correction des champs en Majuscule correction du format date vers nombre entier pour le champ date de mise en service
</commit_message>
<xml_diff>
--- a/exemple-valide.xlsx
+++ b/exemple-valide.xlsx
@@ -94,10 +94,10 @@
     <t xml:space="preserve">46.59698</t>
   </si>
   <si>
-    <t xml:space="preserve">arceau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stationnement non fermé</t>
+    <t xml:space="preserve">ARCEAU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATIONNEMENT NON FERME</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.lpa.fr/se-garer-dans-un-parking/motos-scooters-velos/</t>
@@ -110,13 +110,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="&quot;VRAI&quot;;&quot;VRAI&quot;;&quot;FAUX&quot;"/>
-    <numFmt numFmtId="167" formatCode="YYYY\-MM\-DD"/>
+    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -136,6 +134,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -180,21 +183,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -214,18 +209,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="8.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="54.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="0" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="0" width="12.91"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -290,11 +297,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="0" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="0" t="n">
@@ -345,33 +352,9 @@
       <c r="R2" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="S2" s="0" t="n">
+      <c r="S2" s="1" t="n">
         <v>44091</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Correction des fichiers exemples, champ protection
</commit_message>
<xml_diff>
--- a/exemple-valide.xlsx
+++ b/exemple-valide.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t xml:space="preserve">id_local</t>
   </si>
@@ -100,10 +100,16 @@
     <t xml:space="preserve">STATIONNEMENT NON FERME</t>
   </si>
   <si>
+    <t xml:space="preserve">LIBRE</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.lpa.fr/se-garer-dans-un-parking/motos-scooters-velos/</t>
   </si>
   <si>
     <t xml:space="preserve">Ville de Paris</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-09-17</t>
   </si>
 </sst>
 </file>
@@ -112,9 +118,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -134,11 +140,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -188,8 +189,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -212,7 +213,7 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -224,7 +225,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="28.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="6.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.16"/>
@@ -232,7 +233,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="54.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="0" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="0" width="12.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="10.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="12.96"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -297,7 +299,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>20</v>
       </c>
@@ -328,8 +330,8 @@
       <c r="J2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K2" s="0" t="n">
-        <v>1</v>
+      <c r="K2" s="0" t="s">
+        <v>26</v>
       </c>
       <c r="L2" s="0" t="n">
         <v>0</v>
@@ -338,22 +340,22 @@
         <v>1</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O2" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="S2" s="1" t="n">
-        <v>44091</v>
+        <v>28</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modification formatage cellules .xlsx
</commit_message>
<xml_diff>
--- a/exemple-valide.xlsx
+++ b/exemple-valide.xlsx
@@ -125,6 +125,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -184,8 +185,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -213,21 +218,21 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="M24" activeCellId="0" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="28.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="54.51"/>
@@ -306,7 +311,7 @@
       <c r="B2" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>34172</v>
       </c>
       <c r="D2" s="0" t="s">
@@ -327,16 +332,16 @@
       <c r="I2" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="J2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="K2" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="L2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="M2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="N2" s="0" t="s">
@@ -354,7 +359,7 @@
       <c r="R2" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="S2" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Nouvelle correction type .xlsx
</commit_message>
<xml_diff>
--- a/exemple-valide.xlsx
+++ b/exemple-valide.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t xml:space="preserve">id_local</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t xml:space="preserve">n71729735</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34712</t>
   </si>
   <si>
     <t xml:space="preserve">1.452323</t>
@@ -118,8 +121,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="&quot;VRAI&quot;;&quot;VRAI&quot;;&quot;FAUX&quot;"/>
+    <numFmt numFmtId="165" formatCode="&quot;BOOL&quot;E&quot;AN&quot;"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -186,7 +189,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -195,11 +198,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -223,10 +222,10 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M31" activeCellId="0" sqref="M31"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.32"/>
@@ -316,14 +315,14 @@
       <c r="B2" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="1" t="n">
-        <v>34172</v>
+      <c r="C2" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>8</v>
@@ -332,40 +331,43 @@
         <v>3</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="2" t="b">
+        <v>26</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="2" t="b">
+        <v>27</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="M2" s="2" t="b">
+      <c r="M2" s="1" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O2" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="S2" s="3" t="s">
         <v>29</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nouveau changement type .xlsx
</commit_message>
<xml_diff>
--- a/exemple-valide.xlsx
+++ b/exemple-valide.xlsx
@@ -121,7 +121,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;BOOL&quot;E&quot;AN&quot;"/>
+    <numFmt numFmtId="165" formatCode="&quot;VRAI&quot;;&quot;VRAI&quot;;&quot;FAUX&quot;"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="4">
@@ -222,10 +222,10 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.32"/>
@@ -238,7 +238,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="54.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="0" width="12.13"/>
@@ -336,19 +336,16 @@
       <c r="I2" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="1" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="J2" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K2" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="1" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="L2" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="M2" s="1" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="M2" s="1" t="b">
         <v>1</v>
       </c>
       <c r="N2" s="0" t="s">

</xml_diff>